<commit_message>
Threaded v Unthreaded Optimized tests
</commit_message>
<xml_diff>
--- a/Assignment/Ray Tracer Stats.xlsx
+++ b/Assignment/Ray Tracer Stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d012120g.STUDENT\Documents\RayTracer\Assignment\RayTracerFramework - 16012120\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d012120g\Documents\RayTracer\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC1EF2ED-022D-4EC5-9A2A-06FD36BB7351}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FE083A-D198-4B7F-8819-CFD0DFFCE17F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{317DAF21-ABA5-4838-8D22-3C097FA217EF}"/>
   </bookViews>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>old</t>
   </si>
@@ -70,6 +69,27 @@
   </si>
   <si>
     <t>10th</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>1080p Resolution</t>
+  </si>
+  <si>
+    <t>4k Resolution</t>
+  </si>
+  <si>
+    <t>optimized (milliseconds)</t>
+  </si>
+  <si>
+    <t>threaded optimized (milliseconds)</t>
+  </si>
+  <si>
+    <t>% speed improvement</t>
   </si>
 </sst>
 </file>
@@ -324,6 +344,1212 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Comparison of code structures 1080p Resolution </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1110067804024497"/>
+          <c:y val="4.1666666666666664E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>optimized (milliseconds)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$G$3:$G$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1st</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2nd</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3rd</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4th</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5th</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30852</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31368</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30866</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-25E0-4C17-816A-F006576EFCAB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>threaded optimized (milliseconds)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$G$3:$G$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1st</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2nd</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3rd</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4th</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5th</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$3:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>17959</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18538</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19103</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18309</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17490</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-25E0-4C17-816A-F006576EFCAB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="656648832"/>
+        <c:axId val="656647192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="656648832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> No.</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="656647192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="656647192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time Taken To Render All Frrames</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="656648832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82B395AB-6267-4576-9F4C-19099983B812}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,18 +1849,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0714917-B1DD-4CEB-B305-16418493C008}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -642,8 +1875,14 @@
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -653,8 +1892,26 @@
       <c r="C2" s="4">
         <v>1.4586200000000001E-2</v>
       </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -664,8 +1921,26 @@
       <c r="C3" s="4">
         <v>3.0931700000000001E-3</v>
       </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>30852</v>
+      </c>
+      <c r="I3">
+        <v>17959</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>115263</v>
+      </c>
+      <c r="M3">
+        <v>62244</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -675,8 +1950,26 @@
       <c r="C4" s="4">
         <v>3.4905499999999998E-3</v>
       </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>31368</v>
+      </c>
+      <c r="I4">
+        <v>18538</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>119228</v>
+      </c>
+      <c r="M4">
+        <v>62235</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -686,8 +1979,26 @@
       <c r="C5" s="4">
         <v>3.6270299999999998E-3</v>
       </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>31839</v>
+      </c>
+      <c r="I5">
+        <v>19103</v>
+      </c>
+      <c r="K5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>113908</v>
+      </c>
+      <c r="M5">
+        <v>53400</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -697,8 +2008,26 @@
       <c r="C6" s="4">
         <v>2.6827700000000001E-3</v>
       </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>30299</v>
+      </c>
+      <c r="I6">
+        <v>18309</v>
+      </c>
+      <c r="K6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <v>113043</v>
+      </c>
+      <c r="M6">
+        <v>64325</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -708,8 +2037,26 @@
       <c r="C7" s="4">
         <v>2.2526E-3</v>
       </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>30866</v>
+      </c>
+      <c r="I7">
+        <v>17490</v>
+      </c>
+      <c r="K7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <v>116139</v>
+      </c>
+      <c r="M7">
+        <v>61585</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -719,8 +2066,30 @@
       <c r="C8" s="4">
         <v>3.7842399999999999E-3</v>
       </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <f>SUM(H3:H7)/COUNT(H3:H7)</f>
+        <v>31044.799999999999</v>
+      </c>
+      <c r="I8">
+        <f>SUM(I3:I7)/COUNT(I3:I7)</f>
+        <v>18279.8</v>
+      </c>
+      <c r="K8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ref="J8:M8" si="0">SUM(L3:L7)/COUNT(L3:L7)</f>
+        <v>115516.2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>60757.8</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -731,7 +2100,7 @@
         <v>4.2693899999999996E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -741,8 +2110,30 @@
       <c r="C10" s="4">
         <v>6.1964699999999999E-3</v>
       </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <f>H8/1000</f>
+        <v>31.044799999999999</v>
+      </c>
+      <c r="I10">
+        <f>I8/1000</f>
+        <v>18.279799999999998</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10">
+        <f>L8/1000</f>
+        <v>115.5162</v>
+      </c>
+      <c r="M10">
+        <f>M8/1000</f>
+        <v>60.757800000000003</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
@@ -753,7 +2144,7 @@
         <v>2.9523499999999999E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>2</v>
       </c>
@@ -765,13 +2156,27 @@
         <f>SUM(C2:C11)/10</f>
         <v>4.6934769999999997E-3</v>
       </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E13">
         <v>1146.3800000000001</v>
       </c>
+      <c r="G13">
+        <f>(I8/H8)*100</f>
+        <v>58.882002783074782</v>
+      </c>
+      <c r="K13">
+        <f>(M8/L8)*100</f>
+        <v>52.596778633646188</v>
+      </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="13">
         <f>(C12/B12)*100</f>
         <v>9.6420756068980359E-2</v>
@@ -784,7 +2189,7 @@
         <v>16055.2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C15">
         <f>E14/E13</f>
         <v>14.005129189274061</v>
@@ -795,5 +2200,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>